<commit_message>
docs(): updated backlog with project details
</commit_message>
<xml_diff>
--- a/Product Documents/Product_Backlog.xlsx
+++ b/Product Documents/Product_Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfallahi\OneDrive - University of North Carolina at Charlotte\Teaching\Assignments\6 - Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4C0384B11AF22A34/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_873C540266554DD0153A27FC6AB877793E71760B" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{054B7034-C590-491C-8BE4-13B81AE24F54}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{8DB40486-A4CE-4C8C-BB1A-575B7FDDAA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48A5B08E-F9C9-4DF0-878C-85831BA58114}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11080" yWindow="0" windowWidth="14610" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>ITSC-3155 Software Engineering</t>
   </si>
@@ -46,9 +46,6 @@
     <t>SPRINT #</t>
   </si>
   <si>
-    <t>Feature 1</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -58,16 +55,40 @@
     <t>No</t>
   </si>
   <si>
-    <t>Feature 2</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>Feature 3</t>
-  </si>
-  <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Guest Checkout</t>
+  </si>
+  <si>
+    <t>Detailed Menu Exploration</t>
+  </si>
+  <si>
+    <t>Order Tracking and Type Identification</t>
+  </si>
+  <si>
+    <t>Payment Processing</t>
+  </si>
+  <si>
+    <t>Live Order Status</t>
+  </si>
+  <si>
+    <t>Customer Feedback and Rating</t>
+  </si>
+  <si>
+    <t>Promotional Code Generator</t>
+  </si>
+  <si>
+    <t>Collect and Use Data of Orders Over Time</t>
+  </si>
+  <si>
+    <t>Readable Use Documentation</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -189,16 +210,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -210,7 +227,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,38 +452,39 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="13">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -483,137 +504,209 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="12.5">
       <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="12.5">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="12.5">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="12.5">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.5">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3">
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4"/>
+    <row r="9" spans="1:6" ht="12.5">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.5">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="9">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="12.5">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="12.5">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="12.5">
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="4"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="12.5">
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="4"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="12.5">
+      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>